<commit_message>
update notes and data_dict
</commit_message>
<xml_diff>
--- a/data_dictionary/data_dictionary_bosch.xlsx
+++ b/data_dictionary/data_dictionary_bosch.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin/code/starthack19/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2929FD6C-D8DB-F740-8F02-9A7E87174B24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98892FBE-CFDD-084B-A7F8-6EAC2B71AFB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9A91A77-53F7-3D45-8B3D-165BF87F6333}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{C9A91A77-53F7-3D45-8B3D-165BF87F6333}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="car data" sheetId="1" r:id="rId1"/>
+    <sheet name="empatica" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="169">
   <si>
     <t xml:space="preserve">Signal name </t>
   </si>
@@ -497,6 +498,111 @@
   </si>
   <si>
     <t>Driver interaction - basic</t>
+  </si>
+  <si>
+    <t>automated route detection</t>
+  </si>
+  <si>
+    <t>automated route detection, traffic</t>
+  </si>
+  <si>
+    <t>traffic</t>
+  </si>
+  <si>
+    <t>available seats</t>
+  </si>
+  <si>
+    <t>traffic, stress</t>
+  </si>
+  <si>
+    <t>mood, stress</t>
+  </si>
+  <si>
+    <t>Stress Data if ride or not</t>
+  </si>
+  <si>
+    <t>Electrodermal activity</t>
+  </si>
+  <si>
+    <t>EDA</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Abbreviation</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Measures the change in skin conductance, which changes when you sweat</t>
+  </si>
+  <si>
+    <t>You can detect physical arousals of any kind</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photoplethysmography sensors </t>
+  </si>
+  <si>
+    <t>PPG</t>
+  </si>
+  <si>
+    <t>illuminates the skin and measures changes in light absorption, which gives you the heart rate</t>
+  </si>
+  <si>
+    <t>Heart rate (beats per minute)</t>
+  </si>
+  <si>
+    <t>HR (BPM)</t>
+  </si>
+  <si>
+    <t>Heart rate</t>
+  </si>
+  <si>
+    <t>detect stress, e.g. from high heart rate</t>
+  </si>
+  <si>
+    <t>temperature signal</t>
+  </si>
+  <si>
+    <t>Skin temperature</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>3D- acceleration meter</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>BVP</t>
+  </si>
+  <si>
+    <t>Beats per minute</t>
+  </si>
+  <si>
+    <t>degree celsius</t>
+  </si>
+  <si>
+    <t>G = 9.8 m/s^2</t>
+  </si>
+  <si>
+    <t>if you are waving a lot, you might be stressed</t>
+  </si>
+  <si>
+    <t>Use the driving simulator from Autosense to collect some data</t>
+  </si>
+  <si>
+    <t>we have one signal, no 3D dimensions</t>
+  </si>
+  <si>
+    <t>Data for Demo: Drive around with the car</t>
   </si>
 </sst>
 </file>
@@ -579,17 +685,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -598,9 +695,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -617,6 +711,25 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3697,7 +3810,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>2781300</xdr:colOff>
       <xdr:row>195</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>116840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3729,6 +3842,372 @@
         <a:xfrm>
           <a:off x="914400" y="37871400"/>
           <a:ext cx="4267200" cy="1955800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>201</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52" descr="page4image4285541440">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3672C89E-DCE2-F74E-B5C1-0550FEE0A445}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="43713400"/>
+          <a:ext cx="469900" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53" descr="page4image4285541712">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B61529B-D23C-6F49-A30B-D9A9E41D3CD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="43916600"/>
+          <a:ext cx="228600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54" descr="page4image4285541984">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0553F4A9-7E84-0844-A56A-EC3EE47E904B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="241300" y="43916600"/>
+          <a:ext cx="165100" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55" descr="page4image4285542320">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF96CDE-FE8C-2947-9D91-9292AAAEFF5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="419100" y="43916600"/>
+          <a:ext cx="482600" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>2794000</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3352800</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 57" descr="page4image4285543008">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93FC70E9-CB09-BD48-B3F1-66EAF2FB5786}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5194300" y="43916600"/>
+          <a:ext cx="558800" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2540</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>738050</xdr:colOff>
+      <xdr:row>226</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58" descr="page4image4285543280">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A144BBCE-C032-7B47-8045-D96077EB4FE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2540" y="43627040"/>
+          <a:ext cx="7136310" cy="5191760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4047,1376 +4526,1410 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BE75CC7-764F-714D-8AD9-E1D1651D56AC}">
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:E216"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="31.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="52.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="57.33203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="31.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="57.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="12" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="7"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:5" ht="17">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:5" ht="17">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="10"/>
+      <c r="D8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:5" ht="17">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="D13" s="3"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:5" ht="17">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="20" spans="1:5" ht="18">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:5" ht="17">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="4" t="s">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="10"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="D28" s="10"/>
     </row>
     <row r="29" spans="1:5" ht="17">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="5" t="s">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="10"/>
     </row>
     <row r="30" spans="1:5" ht="17">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="4" t="s">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="D31" s="3"/>
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="D31" s="10"/>
     </row>
     <row r="32" spans="1:5" ht="17">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="4" t="s">
+      <c r="D32" s="10"/>
+      <c r="E32" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
+      <c r="A33" s="9"/>
+      <c r="B33" s="9"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
     </row>
     <row r="34" spans="1:5" ht="17">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D34" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E34" s="4" t="s">
+      <c r="E34" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="38" spans="1:5" ht="18">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="1" t="s">
+      <c r="D40" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D42" s="9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2" t="s">
+    <row r="43" spans="1:5" ht="17">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="17">
+      <c r="A44" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="9" t="s">
         <v>42</v>
       </c>
+      <c r="E44" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="2" t="s">
+      <c r="A45" s="9"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9"/>
+    </row>
+    <row r="46" spans="1:5" ht="17">
+      <c r="A46" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
     </row>
     <row r="48" spans="1:5" ht="17">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="34">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="5" t="s">
+    <row r="49" spans="1:5" ht="34">
+      <c r="A49" s="9"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="2" t="s">
+    <row r="50" spans="1:5">
+      <c r="A50" s="9"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="9" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:4" ht="17">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="5" t="s">
+    <row r="52" spans="1:5">
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="D52" s="9"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="D53" s="9"/>
+    </row>
+    <row r="54" spans="1:5" ht="17">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="D55" s="2"/>
-    </row>
-    <row r="57" spans="1:4" ht="18">
-      <c r="A57" s="6" t="s">
+      <c r="D54" s="9"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="D55" s="9"/>
+    </row>
+    <row r="57" spans="1:5" ht="18">
+      <c r="A57" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="1" t="s">
+      <c r="E57" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" ht="17">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="8" t="s">
+    <row r="60" spans="1:5">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11"/>
+      <c r="D60" s="11"/>
+    </row>
+    <row r="61" spans="1:5" ht="17">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11"/>
+      <c r="C61" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="1"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="D62" s="1"/>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="2" t="s">
+      <c r="D61" s="11"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="11"/>
+      <c r="B63" s="11"/>
+      <c r="D63" s="11"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C64" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D64" s="3"/>
-    </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="2" t="s">
+      <c r="D64" s="10"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="10"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="9"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="10"/>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C67" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="A69" s="2" t="s">
+      <c r="D67" s="10"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="10"/>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="3"/>
-    </row>
-    <row r="70" spans="1:4">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="71" spans="1:4" ht="17">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="5" t="s">
+      <c r="D69" s="10"/>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="D70" s="10"/>
+    </row>
+    <row r="71" spans="1:5" ht="17">
+      <c r="A71" s="9"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="D72" s="3"/>
-    </row>
-    <row r="73" spans="1:4">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:4">
-      <c r="A74" s="2" t="s">
+      <c r="D71" s="10"/>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="9"/>
+      <c r="B72" s="9"/>
+      <c r="D72" s="10"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="D73" s="10"/>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="C74" s="2" t="s">
+      <c r="C74" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D74" s="3"/>
-    </row>
-    <row r="75" spans="1:4">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
-    </row>
-    <row r="76" spans="1:4">
-      <c r="A76" s="2" t="s">
+      <c r="D74" s="10"/>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="9"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
+      <c r="D75" s="10"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D76" s="3"/>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="D77" s="3"/>
-    </row>
-    <row r="78" spans="1:4" ht="17">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="5" t="s">
+      <c r="D76" s="10"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="9"/>
+      <c r="B77" s="9"/>
+      <c r="D77" s="10"/>
+    </row>
+    <row r="78" spans="1:5" ht="17">
+      <c r="A78" s="9"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D78" s="3"/>
-    </row>
-    <row r="79" spans="1:4">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="D79" s="3"/>
-    </row>
-    <row r="80" spans="1:4">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="1:4" ht="17">
-      <c r="A81" s="2" t="s">
+      <c r="D78" s="10"/>
+    </row>
+    <row r="79" spans="1:5" ht="17">
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="9"/>
+      <c r="B80" s="9"/>
+      <c r="D80" s="10"/>
+    </row>
+    <row r="81" spans="1:5" ht="17">
+      <c r="A81" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="34">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="5" t="s">
+    <row r="82" spans="1:5" ht="34">
+      <c r="A82" s="9"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" s="2" t="s">
+    <row r="83" spans="1:5">
+      <c r="A83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="9"/>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B84" s="2" t="s">
+      <c r="B84" s="9" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-    </row>
-    <row r="86" spans="1:4" ht="17">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="5" t="s">
+    <row r="85" spans="1:5">
+      <c r="A85" s="9"/>
+      <c r="B85" s="9"/>
+    </row>
+    <row r="86" spans="1:5" ht="17">
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-    </row>
-    <row r="88" spans="1:4">
-      <c r="A88" s="2" t="s">
+    <row r="87" spans="1:5">
+      <c r="A87" s="9"/>
+      <c r="B87" s="9"/>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:4">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="D89" s="3"/>
-    </row>
-    <row r="90" spans="1:4" ht="17">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="5" t="s">
+      <c r="D88" s="10"/>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="D89" s="10"/>
+    </row>
+    <row r="90" spans="1:5" ht="17">
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="1:4">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="D91" s="3"/>
-    </row>
-    <row r="92" spans="1:4">
-      <c r="A92" s="2" t="s">
+      <c r="D90" s="10"/>
+      <c r="E90" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="9"/>
+      <c r="B91" s="9"/>
+      <c r="D91" s="10"/>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="B92" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="D92" s="3"/>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="D93" s="3"/>
-    </row>
-    <row r="94" spans="1:4" ht="17">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="5" t="s">
+      <c r="D92" s="10"/>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="9"/>
+      <c r="B93" s="9"/>
+      <c r="D93" s="10"/>
+    </row>
+    <row r="94" spans="1:5" ht="17">
+      <c r="A94" s="9"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D94" s="3"/>
-    </row>
-    <row r="95" spans="1:4">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="D95" s="3"/>
-    </row>
-    <row r="96" spans="1:4">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="D96" s="3"/>
-    </row>
-    <row r="97" spans="1:4">
-      <c r="A97" s="2" t="s">
+      <c r="D94" s="10"/>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="9"/>
+      <c r="B95" s="9"/>
+      <c r="D95" s="10"/>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="9"/>
+      <c r="B96" s="9"/>
+      <c r="D96" s="10"/>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="B97" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C97" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="1:4">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="3"/>
-    </row>
-    <row r="99" spans="1:4">
-      <c r="A99" s="2" t="s">
+      <c r="D97" s="10"/>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="9"/>
+      <c r="B98" s="9"/>
+      <c r="C98" s="9"/>
+      <c r="D98" s="10"/>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B99" s="2" t="s">
+      <c r="B99" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C99" s="2" t="s">
+      <c r="C99" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D99" s="2" t="s">
+      <c r="D99" s="9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
-    </row>
-    <row r="102" spans="1:4" ht="18">
-      <c r="A102" s="6" t="s">
+    <row r="100" spans="1:5">
+      <c r="A100" s="9"/>
+      <c r="B100" s="9"/>
+      <c r="C100" s="9"/>
+      <c r="D100" s="9"/>
+    </row>
+    <row r="102" spans="1:5" ht="18">
+      <c r="A102" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="1" t="s">
+    <row r="104" spans="1:5">
+      <c r="A104" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C104" s="1" t="s">
+      <c r="C104" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D104" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="A105" s="1"/>
-      <c r="B105" s="1"/>
-      <c r="C105" s="1"/>
-      <c r="D105" s="1"/>
-    </row>
-    <row r="106" spans="1:4">
-      <c r="A106" s="2" t="s">
+    <row r="105" spans="1:5">
+      <c r="A105" s="11"/>
+      <c r="B105" s="11"/>
+      <c r="C105" s="11"/>
+      <c r="D105" s="11"/>
+    </row>
+    <row r="106" spans="1:5">
+      <c r="A106" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C106" s="2" t="s">
+      <c r="C106" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-    </row>
-    <row r="109" spans="1:4" ht="34">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="5" t="s">
+    <row r="107" spans="1:5">
+      <c r="A107" s="9"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9"/>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="A108" s="9"/>
+      <c r="B108" s="9"/>
+      <c r="C108" s="9"/>
+    </row>
+    <row r="109" spans="1:5" ht="51">
+      <c r="A109" s="9"/>
+      <c r="B109" s="9"/>
+      <c r="C109" s="9"/>
+      <c r="D109" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-    </row>
-    <row r="111" spans="1:4">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-    </row>
-    <row r="112" spans="1:4">
-      <c r="A112" s="2" t="s">
+    <row r="110" spans="1:5" ht="17">
+      <c r="A110" s="9"/>
+      <c r="B110" s="9"/>
+      <c r="C110" s="9"/>
+      <c r="E110" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="A111" s="9"/>
+      <c r="B111" s="9"/>
+      <c r="C111" s="9"/>
+    </row>
+    <row r="112" spans="1:5" ht="17">
+      <c r="A112" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="2"/>
-      <c r="B113" s="2"/>
-    </row>
-    <row r="114" spans="1:4">
-      <c r="A114" s="2" t="s">
+      <c r="E112" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
+      <c r="A113" s="9"/>
+      <c r="B113" s="9"/>
+    </row>
+    <row r="114" spans="1:5" ht="17">
+      <c r="A114" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B114" s="2" t="s">
+      <c r="B114" s="9" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
-      <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
-    </row>
-    <row r="116" spans="1:4">
-      <c r="A116" s="2" t="s">
+      <c r="E114" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
+      <c r="A115" s="9"/>
+      <c r="B115" s="9"/>
+    </row>
+    <row r="116" spans="1:5">
+      <c r="A116" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="9" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
-      <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
-    </row>
-    <row r="118" spans="1:4">
-      <c r="A118" s="2" t="s">
+    <row r="117" spans="1:5" ht="17">
+      <c r="A117" s="9"/>
+      <c r="B117" s="9"/>
+      <c r="E117" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="17">
+      <c r="A118" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="9" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-    </row>
-    <row r="121" spans="1:4" ht="18">
-      <c r="A121" s="6" t="s">
+      <c r="E118" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
+      <c r="A119" s="9"/>
+      <c r="B119" s="9"/>
+    </row>
+    <row r="121" spans="1:5" ht="18">
+      <c r="A121" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
-      <c r="A123" s="1" t="s">
+    <row r="123" spans="1:5">
+      <c r="A123" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B123" s="1" t="s">
+      <c r="B123" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="D123" s="11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
-      <c r="A124" s="1"/>
-      <c r="B124" s="1"/>
-      <c r="D124" s="1"/>
-    </row>
-    <row r="125" spans="1:4" ht="17">
-      <c r="A125" s="1"/>
-      <c r="B125" s="1"/>
-      <c r="C125" s="8" t="s">
+    <row r="124" spans="1:5">
+      <c r="A124" s="11"/>
+      <c r="B124" s="11"/>
+      <c r="D124" s="11"/>
+    </row>
+    <row r="125" spans="1:5" ht="17">
+      <c r="A125" s="11"/>
+      <c r="B125" s="11"/>
+      <c r="C125" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D125" s="1"/>
-    </row>
-    <row r="126" spans="1:4">
-      <c r="A126" s="1"/>
-      <c r="B126" s="1"/>
-      <c r="D126" s="1"/>
-    </row>
-    <row r="127" spans="1:4">
-      <c r="A127" s="2" t="s">
+      <c r="D125" s="11"/>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="11"/>
+      <c r="B126" s="11"/>
+      <c r="D126" s="11"/>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="B127" s="2" t="s">
+      <c r="B127" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D127" s="2" t="s">
+      <c r="D127" s="9" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="D128" s="2"/>
+    <row r="128" spans="1:5">
+      <c r="A128" s="9"/>
+      <c r="B128" s="9"/>
+      <c r="D128" s="9"/>
     </row>
     <row r="129" spans="1:4" ht="17">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="5" t="s">
+      <c r="A129" s="9"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D129" s="2"/>
+      <c r="D129" s="9"/>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="D130" s="2"/>
+      <c r="A130" s="9"/>
+      <c r="B130" s="9"/>
+      <c r="D130" s="9"/>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
+      <c r="A132" s="9"/>
+      <c r="B132" s="9"/>
     </row>
     <row r="133" spans="1:4" ht="17">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="5" t="s">
+      <c r="A133" s="9"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
+      <c r="A135" s="9"/>
+      <c r="B135" s="9"/>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C136" s="2" t="s">
+      <c r="C136" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
+      <c r="A137" s="9"/>
+      <c r="B137" s="9"/>
+      <c r="C137" s="9"/>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-    </row>
-    <row r="139" spans="1:4">
-      <c r="A139" s="2" t="s">
+      <c r="A138" s="9"/>
+      <c r="B138" s="9"/>
+      <c r="C138" s="9"/>
+    </row>
+    <row r="139" spans="1:4" ht="17">
+      <c r="A139" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B139" s="2" t="s">
+      <c r="B139" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C139" s="2" t="s">
+      <c r="C139" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="D139" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
+      <c r="A140" s="9"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
+      <c r="A141" s="9"/>
+      <c r="B141" s="9"/>
+      <c r="C141" s="9"/>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C142" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="9"/>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B144" s="9" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
+      <c r="A145" s="9"/>
+      <c r="B145" s="9"/>
     </row>
     <row r="146" spans="1:4" ht="17">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="5" t="s">
+      <c r="A146" s="9"/>
+      <c r="B146" s="9"/>
+      <c r="C146" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
+      <c r="A147" s="9"/>
+      <c r="B147" s="9"/>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="2" t="s">
+      <c r="A148" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B148" s="2" t="s">
+      <c r="B148" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
+      <c r="A149" s="9"/>
+      <c r="B149" s="9"/>
     </row>
     <row r="150" spans="1:4" ht="17">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="5" t="s">
+      <c r="A150" s="9"/>
+      <c r="B150" s="9"/>
+      <c r="C150" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
+      <c r="A151" s="9"/>
+      <c r="B151" s="9"/>
     </row>
     <row r="152" spans="1:4">
-      <c r="A152" s="2" t="s">
+      <c r="A152" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="9" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c r="A153" s="2"/>
-      <c r="B153" s="2"/>
+      <c r="A153" s="9"/>
+      <c r="B153" s="9"/>
     </row>
     <row r="154" spans="1:4" ht="17">
-      <c r="A154" s="2"/>
-      <c r="B154" s="2"/>
-      <c r="C154" s="5" t="s">
+      <c r="A154" s="9"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:4">
-      <c r="A155" s="2"/>
-      <c r="B155" s="2"/>
+      <c r="A155" s="9"/>
+      <c r="B155" s="9"/>
     </row>
     <row r="156" spans="1:4">
-      <c r="A156" s="2"/>
-      <c r="B156" s="2"/>
+      <c r="A156" s="9"/>
+      <c r="B156" s="9"/>
     </row>
     <row r="157" spans="1:4">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C157" s="2" t="s">
+      <c r="C157" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D157" s="3"/>
+      <c r="D157" s="10"/>
     </row>
     <row r="158" spans="1:4">
-      <c r="A158" s="2"/>
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
-      <c r="D158" s="3"/>
+      <c r="A158" s="9"/>
+      <c r="B158" s="9"/>
+      <c r="C158" s="9"/>
+      <c r="D158" s="10"/>
     </row>
     <row r="160" spans="1:4" ht="18">
-      <c r="A160" s="6" t="s">
+      <c r="A160" s="3" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c r="A162" s="1" t="s">
+      <c r="A162" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B162" s="1" t="s">
+      <c r="B162" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D162" s="1" t="s">
+      <c r="D162" s="11" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:4">
-      <c r="A163" s="1"/>
-      <c r="B163" s="1"/>
-      <c r="D163" s="1"/>
+      <c r="A163" s="11"/>
+      <c r="B163" s="11"/>
+      <c r="D163" s="11"/>
     </row>
     <row r="164" spans="1:4" ht="17">
-      <c r="A164" s="1"/>
-      <c r="B164" s="1"/>
-      <c r="C164" s="8" t="s">
+      <c r="A164" s="11"/>
+      <c r="B164" s="11"/>
+      <c r="C164" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D164" s="1"/>
+      <c r="D164" s="11"/>
     </row>
     <row r="165" spans="1:4">
-      <c r="A165" s="1"/>
-      <c r="B165" s="1"/>
-      <c r="D165" s="1"/>
+      <c r="A165" s="11"/>
+      <c r="B165" s="11"/>
+      <c r="D165" s="11"/>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="1"/>
-      <c r="B166" s="1"/>
-      <c r="D166" s="1"/>
+      <c r="A166" s="11"/>
+      <c r="B166" s="11"/>
+      <c r="D166" s="11"/>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="2" t="s">
+      <c r="A167" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B167" s="2" t="s">
+      <c r="B167" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="C167" s="2" t="s">
+      <c r="C167" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D167" s="3"/>
+      <c r="D167" s="10"/>
     </row>
     <row r="168" spans="1:4">
-      <c r="A168" s="2"/>
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
-      <c r="D168" s="3"/>
+      <c r="A168" s="9"/>
+      <c r="B168" s="9"/>
+      <c r="C168" s="9"/>
+      <c r="D168" s="10"/>
     </row>
     <row r="169" spans="1:4">
-      <c r="A169" s="2" t="s">
+      <c r="A169" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B169" s="2" t="s">
+      <c r="B169" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C169" s="2" t="s">
+      <c r="C169" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D169" s="3"/>
+      <c r="D169" s="10"/>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="2"/>
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-      <c r="D170" s="3"/>
+      <c r="A170" s="9"/>
+      <c r="B170" s="9"/>
+      <c r="C170" s="9"/>
+      <c r="D170" s="10"/>
     </row>
     <row r="171" spans="1:4">
-      <c r="A171" s="2" t="s">
+      <c r="A171" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B171" s="2" t="s">
+      <c r="B171" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="C171" s="2" t="s">
+      <c r="C171" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D171" s="3"/>
+      <c r="D171" s="10"/>
     </row>
     <row r="172" spans="1:4">
-      <c r="A172" s="2"/>
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
-      <c r="D172" s="3"/>
+      <c r="A172" s="9"/>
+      <c r="B172" s="9"/>
+      <c r="C172" s="9"/>
+      <c r="D172" s="10"/>
     </row>
     <row r="173" spans="1:4">
-      <c r="A173" s="2" t="s">
+      <c r="A173" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C173" s="2" t="s">
+      <c r="C173" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D173" s="3"/>
+      <c r="D173" s="10"/>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="2"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="3"/>
+      <c r="A174" s="9"/>
+      <c r="B174" s="9"/>
+      <c r="C174" s="9"/>
+      <c r="D174" s="10"/>
     </row>
     <row r="176" spans="1:4" ht="52">
-      <c r="A176" s="9" t="s">
+      <c r="A176" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="178" spans="1:1" ht="19">
-      <c r="A178" s="10" t="s">
+    <row r="178" spans="1:3" ht="19">
+      <c r="A178" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="179" spans="1:1" ht="46">
-      <c r="A179" s="11" t="s">
+    <row r="179" spans="1:3" ht="46">
+      <c r="A179" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="181" spans="1:1">
-      <c r="A181" s="12" t="s">
+    <row r="181" spans="1:3">
+      <c r="A181" s="8" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="183" spans="1:1" ht="19">
-      <c r="A183" s="10" t="s">
+    <row r="183" spans="1:3" ht="19">
+      <c r="A183" s="6" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="184" spans="1:1" ht="46">
-      <c r="A184" s="11" t="s">
+    <row r="184" spans="1:3" ht="46">
+      <c r="A184" s="7" t="s">
         <v>129</v>
       </c>
+    </row>
+    <row r="187" spans="1:3" ht="17">
+      <c r="C187" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="18">
+      <c r="A199" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4">
+      <c r="A200" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4">
+      <c r="A201"/>
+    </row>
+    <row r="202" spans="1:4">
+      <c r="A202"/>
+    </row>
+    <row r="203" spans="1:4">
+      <c r="A203"/>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204"/>
+    </row>
+    <row r="205" spans="1:4">
+      <c r="A205"/>
+    </row>
+    <row r="206" spans="1:4" ht="17">
+      <c r="A206"/>
+      <c r="D206" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4">
+      <c r="A207"/>
+    </row>
+    <row r="208" spans="1:4">
+      <c r="A208"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216"/>
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="A173:A174"/>
-    <mergeCell ref="B173:B174"/>
-    <mergeCell ref="C173:C174"/>
-    <mergeCell ref="D173:D174"/>
-    <mergeCell ref="A169:A170"/>
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="C169:C170"/>
-    <mergeCell ref="D169:D170"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="B171:B172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="D171:D172"/>
-    <mergeCell ref="A162:A166"/>
-    <mergeCell ref="B162:B166"/>
-    <mergeCell ref="D162:D166"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B167:B168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="D167:D168"/>
-    <mergeCell ref="A152:A156"/>
-    <mergeCell ref="B152:B156"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="A144:A147"/>
-    <mergeCell ref="B144:B147"/>
-    <mergeCell ref="A148:A151"/>
-    <mergeCell ref="B148:B151"/>
-    <mergeCell ref="A136:A138"/>
-    <mergeCell ref="B136:B138"/>
-    <mergeCell ref="C136:C138"/>
-    <mergeCell ref="A139:A141"/>
-    <mergeCell ref="B139:B141"/>
-    <mergeCell ref="C139:C141"/>
-    <mergeCell ref="D123:D126"/>
-    <mergeCell ref="A127:A130"/>
-    <mergeCell ref="B127:B130"/>
-    <mergeCell ref="D127:D130"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="B131:B135"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="B116:B117"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="B123:B126"/>
-    <mergeCell ref="A106:A111"/>
-    <mergeCell ref="B106:B111"/>
-    <mergeCell ref="C106:C111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="D92:D96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="D76:D80"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="D69:D73"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:C45"/>
@@ -5441,47 +5954,244 @@
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="A51:A55"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="D51:D55"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="D76:D80"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="D69:D73"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="D92:D96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="A106:A111"/>
+    <mergeCell ref="B106:B111"/>
+    <mergeCell ref="C106:C111"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D123:D126"/>
+    <mergeCell ref="A127:A130"/>
+    <mergeCell ref="B127:B130"/>
+    <mergeCell ref="D127:D130"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="B131:B135"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="B123:B126"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="A144:A147"/>
+    <mergeCell ref="B144:B147"/>
+    <mergeCell ref="A148:A151"/>
+    <mergeCell ref="B148:B151"/>
+    <mergeCell ref="A136:A138"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="C136:C138"/>
+    <mergeCell ref="A139:A141"/>
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="C139:C141"/>
+    <mergeCell ref="A162:A166"/>
+    <mergeCell ref="B162:B166"/>
+    <mergeCell ref="D162:D166"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="B152:B156"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="A173:A174"/>
+    <mergeCell ref="B173:B174"/>
+    <mergeCell ref="C173:C174"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="A169:A170"/>
+    <mergeCell ref="B169:B170"/>
+    <mergeCell ref="C169:C170"/>
+    <mergeCell ref="D169:D170"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="B171:B172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="D171:D172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8216F98-DF56-724A-A913-28E53FD6273C}">
+  <dimension ref="A2:L15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="32.1640625" style="1" customWidth="1"/>
+    <col min="2" max="3" width="13.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" style="1" customWidth="1"/>
+    <col min="6" max="12" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:12" s="15" customFormat="1" ht="17">
+      <c r="A2" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" ht="51">
+      <c r="A3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="68">
+      <c r="A4" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="34">
+      <c r="A5" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="17">
+      <c r="A6" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="34">
+      <c r="A7" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="34">
+      <c r="A12" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="34">
+      <c r="A15" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
notebook for processing all raw data and streaming them to structured csv. Data dict update
</commit_message>
<xml_diff>
--- a/data_dictionary/data_dictionary_bosch.xlsx
+++ b/data_dictionary/data_dictionary_bosch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin/code/starthack19/data_dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98892FBE-CFDD-084B-A7F8-6EAC2B71AFB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FC493C-2197-3047-AF08-99197BAAC5BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{C9A91A77-53F7-3D45-8B3D-165BF87F6333}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="183">
   <si>
     <t xml:space="preserve">Signal name </t>
   </si>
@@ -603,6 +603,48 @@
   </si>
   <si>
     <t>Data for Demo: Drive around with the car</t>
+  </si>
+  <si>
+    <t>Sampling frequency</t>
+  </si>
+  <si>
+    <t>4 Hz</t>
+  </si>
+  <si>
+    <t>64 Hz</t>
+  </si>
+  <si>
+    <t>1Hz</t>
+  </si>
+  <si>
+    <t>32 Hz</t>
+  </si>
+  <si>
+    <t>csv abbreviation</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>TEMP</t>
+  </si>
+  <si>
+    <t>ACC</t>
+  </si>
+  <si>
+    <t>Interbeat Interval</t>
+  </si>
+  <si>
+    <t>IBI</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
+    <t>1 Hz</t>
+  </si>
+  <si>
+    <t>DO NOT USE</t>
   </si>
 </sst>
 </file>
@@ -685,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -711,17 +753,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -730,6 +763,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4547,61 +4592,61 @@
       </c>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="18" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="18"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="10"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="1:5" ht="17">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="17"/>
       <c r="E5" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -4609,20 +4654,20 @@
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="1:5" ht="17">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="16" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -4630,85 +4675,85 @@
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16"/>
     </row>
     <row r="10" spans="1:5">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="10"/>
+      <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:5" ht="17">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="16"/>
+      <c r="B11" s="16"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="16"/>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="17"/>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="9"/>
-      <c r="B13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="16"/>
+      <c r="D13" s="17"/>
     </row>
     <row r="14" spans="1:5" ht="17">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
       <c r="E14" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="16" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
     </row>
     <row r="20" spans="1:5" ht="18">
       <c r="A20" s="3" t="s">
@@ -4716,119 +4761,119 @@
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="9" t="s">
+      <c r="A25" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="17"/>
     </row>
     <row r="26" spans="1:5" ht="17">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="10"/>
+      <c r="D27" s="17"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="16"/>
+      <c r="D28" s="17"/>
     </row>
     <row r="29" spans="1:5" ht="17">
-      <c r="A29" s="9"/>
-      <c r="B29" s="9"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="16"/>
       <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="17"/>
     </row>
     <row r="30" spans="1:5" ht="17">
-      <c r="A30" s="9"/>
-      <c r="B30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="16"/>
+      <c r="B30" s="16"/>
+      <c r="D30" s="17"/>
       <c r="E30" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="16"/>
+      <c r="B31" s="16"/>
+      <c r="D31" s="17"/>
     </row>
     <row r="32" spans="1:5" ht="17">
-      <c r="A32" s="9" t="s">
+      <c r="A32" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="1" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="16"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
     </row>
     <row r="34" spans="1:5" ht="17">
-      <c r="A34" s="9" t="s">
+      <c r="A34" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D34" s="9" t="s">
+      <c r="D34" s="16" t="s">
         <v>35</v>
       </c>
       <c r="E34" s="1" t="s">
@@ -4836,10 +4881,10 @@
       </c>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="A35" s="16"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
     </row>
     <row r="38" spans="1:5" ht="18">
       <c r="A38" s="3" t="s">
@@ -4847,59 +4892,59 @@
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="11"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="16" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="17">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9"/>
+      <c r="A43" s="16"/>
+      <c r="B43" s="16"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="16"/>
       <c r="E43" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="17">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="C44" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="16" t="s">
         <v>42</v>
       </c>
       <c r="E44" s="1" t="s">
@@ -4907,40 +4952,40 @@
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="9"/>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9"/>
+      <c r="A45" s="16"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
     </row>
     <row r="46" spans="1:5" ht="17">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="10"/>
+      <c r="D46" s="17"/>
       <c r="E46" s="1" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" s="9"/>
-      <c r="B47" s="9"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="10"/>
+      <c r="A47" s="16"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="17"/>
     </row>
     <row r="48" spans="1:5" ht="17">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C48" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D48" s="2" t="s">
@@ -4948,51 +4993,51 @@
       </c>
     </row>
     <row r="49" spans="1:5" ht="34">
-      <c r="A49" s="9"/>
-      <c r="B49" s="9"/>
-      <c r="C49" s="9"/>
+      <c r="A49" s="16"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
       <c r="D49" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="9"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="9"/>
+      <c r="A50" s="16"/>
+      <c r="B50" s="16"/>
+      <c r="C50" s="16"/>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="9" t="s">
+      <c r="A51" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="9"/>
-      <c r="B52" s="9"/>
-      <c r="D52" s="9"/>
+      <c r="A52" s="16"/>
+      <c r="B52" s="16"/>
+      <c r="D52" s="16"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="9"/>
-      <c r="B53" s="9"/>
-      <c r="D53" s="9"/>
+      <c r="A53" s="16"/>
+      <c r="B53" s="16"/>
+      <c r="D53" s="16"/>
     </row>
     <row r="54" spans="1:5" ht="17">
-      <c r="A54" s="9"/>
-      <c r="B54" s="9"/>
+      <c r="A54" s="16"/>
+      <c r="B54" s="16"/>
       <c r="C54" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D54" s="9"/>
+      <c r="D54" s="16"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="9"/>
-      <c r="B55" s="9"/>
-      <c r="D55" s="9"/>
+      <c r="A55" s="16"/>
+      <c r="B55" s="16"/>
+      <c r="D55" s="16"/>
     </row>
     <row r="57" spans="1:5" ht="18">
       <c r="A57" s="3" t="s">
@@ -5003,174 +5048,174 @@
       </c>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D59" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="D60" s="11"/>
+      <c r="A60" s="15"/>
+      <c r="B60" s="15"/>
+      <c r="D60" s="15"/>
     </row>
     <row r="61" spans="1:5" ht="17">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
+      <c r="A61" s="15"/>
+      <c r="B61" s="15"/>
       <c r="C61" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D61" s="11"/>
+      <c r="D61" s="15"/>
     </row>
     <row r="62" spans="1:5">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="D62" s="11"/>
+      <c r="A62" s="15"/>
+      <c r="B62" s="15"/>
+      <c r="D62" s="15"/>
     </row>
     <row r="63" spans="1:5">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
-      <c r="D63" s="11"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="15"/>
+      <c r="D63" s="15"/>
     </row>
     <row r="64" spans="1:5">
-      <c r="A64" s="9" t="s">
+      <c r="A64" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="9" t="s">
+      <c r="C64" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D64" s="10"/>
+      <c r="D64" s="17"/>
     </row>
     <row r="65" spans="1:5">
-      <c r="A65" s="9"/>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="10"/>
+      <c r="A65" s="16"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="16"/>
+      <c r="D65" s="17"/>
     </row>
     <row r="66" spans="1:5">
-      <c r="A66" s="9"/>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9"/>
-      <c r="D66" s="10"/>
+      <c r="A66" s="16"/>
+      <c r="B66" s="16"/>
+      <c r="C66" s="16"/>
+      <c r="D66" s="17"/>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="9" t="s">
+      <c r="A67" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C67" s="9" t="s">
+      <c r="C67" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D67" s="10"/>
+      <c r="D67" s="17"/>
     </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="9"/>
-      <c r="B68" s="9"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="10"/>
+      <c r="A68" s="16"/>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="17"/>
     </row>
     <row r="69" spans="1:5">
-      <c r="A69" s="9" t="s">
+      <c r="A69" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="D69" s="10"/>
+      <c r="D69" s="17"/>
     </row>
     <row r="70" spans="1:5">
-      <c r="A70" s="9"/>
-      <c r="B70" s="9"/>
-      <c r="D70" s="10"/>
+      <c r="A70" s="16"/>
+      <c r="B70" s="16"/>
+      <c r="D70" s="17"/>
     </row>
     <row r="71" spans="1:5" ht="17">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
+      <c r="A71" s="16"/>
+      <c r="B71" s="16"/>
       <c r="C71" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D71" s="10"/>
+      <c r="D71" s="17"/>
     </row>
     <row r="72" spans="1:5">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="D72" s="10"/>
+      <c r="A72" s="16"/>
+      <c r="B72" s="16"/>
+      <c r="D72" s="17"/>
     </row>
     <row r="73" spans="1:5">
-      <c r="A73" s="9"/>
-      <c r="B73" s="9"/>
-      <c r="D73" s="10"/>
+      <c r="A73" s="16"/>
+      <c r="B73" s="16"/>
+      <c r="D73" s="17"/>
     </row>
     <row r="74" spans="1:5">
-      <c r="A74" s="9" t="s">
+      <c r="A74" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B74" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C74" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D74" s="10"/>
+      <c r="D74" s="17"/>
     </row>
     <row r="75" spans="1:5">
-      <c r="A75" s="9"/>
-      <c r="B75" s="9"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="10"/>
+      <c r="A75" s="16"/>
+      <c r="B75" s="16"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="17"/>
     </row>
     <row r="76" spans="1:5">
-      <c r="A76" s="9" t="s">
+      <c r="A76" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D76" s="10"/>
+      <c r="D76" s="17"/>
     </row>
     <row r="77" spans="1:5">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="D77" s="10"/>
+      <c r="A77" s="16"/>
+      <c r="B77" s="16"/>
+      <c r="D77" s="17"/>
     </row>
     <row r="78" spans="1:5" ht="17">
-      <c r="A78" s="9"/>
-      <c r="B78" s="9"/>
+      <c r="A78" s="16"/>
+      <c r="B78" s="16"/>
       <c r="C78" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D78" s="10"/>
+      <c r="D78" s="17"/>
     </row>
     <row r="79" spans="1:5" ht="17">
-      <c r="A79" s="9"/>
-      <c r="B79" s="9"/>
-      <c r="D79" s="10"/>
+      <c r="A79" s="16"/>
+      <c r="B79" s="16"/>
+      <c r="D79" s="17"/>
       <c r="E79" s="1" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:5">
-      <c r="A80" s="9"/>
-      <c r="B80" s="9"/>
-      <c r="D80" s="10"/>
+      <c r="A80" s="16"/>
+      <c r="B80" s="16"/>
+      <c r="D80" s="17"/>
     </row>
     <row r="81" spans="1:5" ht="17">
-      <c r="A81" s="9" t="s">
+      <c r="A81" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="C81" s="9" t="s">
+      <c r="C81" s="16" t="s">
         <v>34</v>
       </c>
       <c r="D81" s="2" t="s">
@@ -5178,140 +5223,140 @@
       </c>
     </row>
     <row r="82" spans="1:5" ht="34">
-      <c r="A82" s="9"/>
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
+      <c r="A82" s="16"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
       <c r="D82" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:5">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
+      <c r="A83" s="16"/>
+      <c r="B83" s="16"/>
+      <c r="C83" s="16"/>
     </row>
     <row r="84" spans="1:5">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="16" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:5">
-      <c r="A85" s="9"/>
-      <c r="B85" s="9"/>
+      <c r="A85" s="16"/>
+      <c r="B85" s="16"/>
     </row>
     <row r="86" spans="1:5" ht="17">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
+      <c r="A86" s="16"/>
+      <c r="B86" s="16"/>
       <c r="C86" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="87" spans="1:5">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
+      <c r="A87" s="16"/>
+      <c r="B87" s="16"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="9" t="s">
+      <c r="A88" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D88" s="10"/>
+      <c r="D88" s="17"/>
     </row>
     <row r="89" spans="1:5">
-      <c r="A89" s="9"/>
-      <c r="B89" s="9"/>
-      <c r="D89" s="10"/>
+      <c r="A89" s="16"/>
+      <c r="B89" s="16"/>
+      <c r="D89" s="17"/>
     </row>
     <row r="90" spans="1:5" ht="17">
-      <c r="A90" s="9"/>
-      <c r="B90" s="9"/>
+      <c r="A90" s="16"/>
+      <c r="B90" s="16"/>
       <c r="C90" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D90" s="10"/>
+      <c r="D90" s="17"/>
       <c r="E90" s="1" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="91" spans="1:5">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="D91" s="10"/>
+      <c r="A91" s="16"/>
+      <c r="B91" s="16"/>
+      <c r="D91" s="17"/>
     </row>
     <row r="92" spans="1:5">
-      <c r="A92" s="9" t="s">
+      <c r="A92" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="D92" s="10"/>
+      <c r="D92" s="17"/>
     </row>
     <row r="93" spans="1:5">
-      <c r="A93" s="9"/>
-      <c r="B93" s="9"/>
-      <c r="D93" s="10"/>
+      <c r="A93" s="16"/>
+      <c r="B93" s="16"/>
+      <c r="D93" s="17"/>
     </row>
     <row r="94" spans="1:5" ht="17">
-      <c r="A94" s="9"/>
-      <c r="B94" s="9"/>
+      <c r="A94" s="16"/>
+      <c r="B94" s="16"/>
       <c r="C94" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D94" s="10"/>
+      <c r="D94" s="17"/>
     </row>
     <row r="95" spans="1:5">
-      <c r="A95" s="9"/>
-      <c r="B95" s="9"/>
-      <c r="D95" s="10"/>
+      <c r="A95" s="16"/>
+      <c r="B95" s="16"/>
+      <c r="D95" s="17"/>
     </row>
     <row r="96" spans="1:5">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
-      <c r="D96" s="10"/>
+      <c r="A96" s="16"/>
+      <c r="B96" s="16"/>
+      <c r="D96" s="17"/>
     </row>
     <row r="97" spans="1:5">
-      <c r="A97" s="9" t="s">
+      <c r="A97" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C97" s="9" t="s">
+      <c r="C97" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D97" s="10"/>
+      <c r="D97" s="17"/>
     </row>
     <row r="98" spans="1:5">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="10"/>
+      <c r="A98" s="16"/>
+      <c r="B98" s="16"/>
+      <c r="C98" s="16"/>
+      <c r="D98" s="17"/>
     </row>
     <row r="99" spans="1:5">
-      <c r="A99" s="9" t="s">
+      <c r="A99" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C99" s="9" t="s">
+      <c r="C99" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="D99" s="9" t="s">
+      <c r="D99" s="16" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:5">
-      <c r="A100" s="9"/>
-      <c r="B100" s="9"/>
-      <c r="C100" s="9"/>
-      <c r="D100" s="9"/>
+      <c r="A100" s="16"/>
+      <c r="B100" s="16"/>
+      <c r="C100" s="16"/>
+      <c r="D100" s="16"/>
     </row>
     <row r="102" spans="1:5" ht="18">
       <c r="A102" s="3" t="s">
@@ -5319,72 +5364,72 @@
       </c>
     </row>
     <row r="104" spans="1:5">
-      <c r="A104" s="11" t="s">
+      <c r="A104" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B104" s="11" t="s">
+      <c r="B104" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C104" s="11" t="s">
+      <c r="C104" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D104" s="11" t="s">
+      <c r="D104" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:5">
-      <c r="A105" s="11"/>
-      <c r="B105" s="11"/>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
+      <c r="A105" s="15"/>
+      <c r="B105" s="15"/>
+      <c r="C105" s="15"/>
+      <c r="D105" s="15"/>
     </row>
     <row r="106" spans="1:5">
-      <c r="A106" s="9" t="s">
+      <c r="A106" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B106" s="9" t="s">
+      <c r="B106" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="C106" s="9" t="s">
+      <c r="C106" s="16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="107" spans="1:5">
-      <c r="A107" s="9"/>
-      <c r="B107" s="9"/>
-      <c r="C107" s="9"/>
+      <c r="A107" s="16"/>
+      <c r="B107" s="16"/>
+      <c r="C107" s="16"/>
     </row>
     <row r="108" spans="1:5">
-      <c r="A108" s="9"/>
-      <c r="B108" s="9"/>
-      <c r="C108" s="9"/>
+      <c r="A108" s="16"/>
+      <c r="B108" s="16"/>
+      <c r="C108" s="16"/>
     </row>
     <row r="109" spans="1:5" ht="51">
-      <c r="A109" s="9"/>
-      <c r="B109" s="9"/>
-      <c r="C109" s="9"/>
+      <c r="A109" s="16"/>
+      <c r="B109" s="16"/>
+      <c r="C109" s="16"/>
       <c r="D109" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="17">
-      <c r="A110" s="9"/>
-      <c r="B110" s="9"/>
-      <c r="C110" s="9"/>
+      <c r="A110" s="16"/>
+      <c r="B110" s="16"/>
+      <c r="C110" s="16"/>
       <c r="E110" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="111" spans="1:5">
-      <c r="A111" s="9"/>
-      <c r="B111" s="9"/>
-      <c r="C111" s="9"/>
+      <c r="A111" s="16"/>
+      <c r="B111" s="16"/>
+      <c r="C111" s="16"/>
     </row>
     <row r="112" spans="1:5" ht="17">
-      <c r="A112" s="9" t="s">
+      <c r="A112" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="B112" s="9" t="s">
+      <c r="B112" s="16" t="s">
         <v>86</v>
       </c>
       <c r="E112" s="1" t="s">
@@ -5392,14 +5437,14 @@
       </c>
     </row>
     <row r="113" spans="1:5">
-      <c r="A113" s="9"/>
-      <c r="B113" s="9"/>
+      <c r="A113" s="16"/>
+      <c r="B113" s="16"/>
     </row>
     <row r="114" spans="1:5" ht="17">
-      <c r="A114" s="9" t="s">
+      <c r="A114" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="B114" s="9" t="s">
+      <c r="B114" s="16" t="s">
         <v>88</v>
       </c>
       <c r="E114" s="1" t="s">
@@ -5407,29 +5452,29 @@
       </c>
     </row>
     <row r="115" spans="1:5">
-      <c r="A115" s="9"/>
-      <c r="B115" s="9"/>
+      <c r="A115" s="16"/>
+      <c r="B115" s="16"/>
     </row>
     <row r="116" spans="1:5">
-      <c r="A116" s="9" t="s">
+      <c r="A116" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B116" s="9" t="s">
+      <c r="B116" s="16" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="17">
-      <c r="A117" s="9"/>
-      <c r="B117" s="9"/>
+      <c r="A117" s="16"/>
+      <c r="B117" s="16"/>
       <c r="E117" s="1" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="118" spans="1:5" ht="17">
-      <c r="A118" s="9" t="s">
+      <c r="A118" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="B118" s="9" t="s">
+      <c r="B118" s="16" t="s">
         <v>92</v>
       </c>
       <c r="E118" s="1" t="s">
@@ -5437,8 +5482,8 @@
       </c>
     </row>
     <row r="119" spans="1:5">
-      <c r="A119" s="9"/>
-      <c r="B119" s="9"/>
+      <c r="A119" s="16"/>
+      <c r="B119" s="16"/>
     </row>
     <row r="121" spans="1:5" ht="18">
       <c r="A121" s="3" t="s">
@@ -5446,119 +5491,119 @@
       </c>
     </row>
     <row r="123" spans="1:5">
-      <c r="A123" s="11" t="s">
+      <c r="A123" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B123" s="11" t="s">
+      <c r="B123" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D123" s="11" t="s">
+      <c r="D123" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:5">
-      <c r="A124" s="11"/>
-      <c r="B124" s="11"/>
-      <c r="D124" s="11"/>
+      <c r="A124" s="15"/>
+      <c r="B124" s="15"/>
+      <c r="D124" s="15"/>
     </row>
     <row r="125" spans="1:5" ht="17">
-      <c r="A125" s="11"/>
-      <c r="B125" s="11"/>
+      <c r="A125" s="15"/>
+      <c r="B125" s="15"/>
       <c r="C125" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D125" s="11"/>
+      <c r="D125" s="15"/>
     </row>
     <row r="126" spans="1:5">
-      <c r="A126" s="11"/>
-      <c r="B126" s="11"/>
-      <c r="D126" s="11"/>
+      <c r="A126" s="15"/>
+      <c r="B126" s="15"/>
+      <c r="D126" s="15"/>
     </row>
     <row r="127" spans="1:5">
-      <c r="A127" s="9" t="s">
+      <c r="A127" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B127" s="9" t="s">
+      <c r="B127" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="D127" s="9" t="s">
+      <c r="D127" s="16" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="128" spans="1:5">
-      <c r="A128" s="9"/>
-      <c r="B128" s="9"/>
-      <c r="D128" s="9"/>
+      <c r="A128" s="16"/>
+      <c r="B128" s="16"/>
+      <c r="D128" s="16"/>
     </row>
     <row r="129" spans="1:4" ht="17">
-      <c r="A129" s="9"/>
-      <c r="B129" s="9"/>
+      <c r="A129" s="16"/>
+      <c r="B129" s="16"/>
       <c r="C129" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D129" s="9"/>
+      <c r="D129" s="16"/>
     </row>
     <row r="130" spans="1:4">
-      <c r="A130" s="9"/>
-      <c r="B130" s="9"/>
-      <c r="D130" s="9"/>
+      <c r="A130" s="16"/>
+      <c r="B130" s="16"/>
+      <c r="D130" s="16"/>
     </row>
     <row r="131" spans="1:4">
-      <c r="A131" s="9" t="s">
+      <c r="A131" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B131" s="9" t="s">
+      <c r="B131" s="16" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:4">
-      <c r="A132" s="9"/>
-      <c r="B132" s="9"/>
+      <c r="A132" s="16"/>
+      <c r="B132" s="16"/>
     </row>
     <row r="133" spans="1:4" ht="17">
-      <c r="A133" s="9"/>
-      <c r="B133" s="9"/>
+      <c r="A133" s="16"/>
+      <c r="B133" s="16"/>
       <c r="C133" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:4">
-      <c r="A134" s="9"/>
-      <c r="B134" s="9"/>
+      <c r="A134" s="16"/>
+      <c r="B134" s="16"/>
     </row>
     <row r="135" spans="1:4">
-      <c r="A135" s="9"/>
-      <c r="B135" s="9"/>
+      <c r="A135" s="16"/>
+      <c r="B135" s="16"/>
     </row>
     <row r="136" spans="1:4">
-      <c r="A136" s="9" t="s">
+      <c r="A136" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B136" s="9" t="s">
+      <c r="B136" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C136" s="9" t="s">
+      <c r="C136" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:4">
-      <c r="A137" s="9"/>
-      <c r="B137" s="9"/>
-      <c r="C137" s="9"/>
+      <c r="A137" s="16"/>
+      <c r="B137" s="16"/>
+      <c r="C137" s="16"/>
     </row>
     <row r="138" spans="1:4">
-      <c r="A138" s="9"/>
-      <c r="B138" s="9"/>
-      <c r="C138" s="9"/>
+      <c r="A138" s="16"/>
+      <c r="B138" s="16"/>
+      <c r="C138" s="16"/>
     </row>
     <row r="139" spans="1:4" ht="17">
-      <c r="A139" s="9" t="s">
+      <c r="A139" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="B139" s="9" t="s">
+      <c r="B139" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="C139" s="9" t="s">
+      <c r="C139" s="16" t="s">
         <v>9</v>
       </c>
       <c r="D139" s="1" t="s">
@@ -5566,121 +5611,121 @@
       </c>
     </row>
     <row r="140" spans="1:4">
-      <c r="A140" s="9"/>
-      <c r="B140" s="9"/>
-      <c r="C140" s="9"/>
+      <c r="A140" s="16"/>
+      <c r="B140" s="16"/>
+      <c r="C140" s="16"/>
     </row>
     <row r="141" spans="1:4">
-      <c r="A141" s="9"/>
-      <c r="B141" s="9"/>
-      <c r="C141" s="9"/>
+      <c r="A141" s="16"/>
+      <c r="B141" s="16"/>
+      <c r="C141" s="16"/>
     </row>
     <row r="142" spans="1:4">
-      <c r="A142" s="9" t="s">
+      <c r="A142" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B142" s="9" t="s">
+      <c r="B142" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="C142" s="9" t="s">
+      <c r="C142" s="16" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:4">
-      <c r="A143" s="9"/>
-      <c r="B143" s="9"/>
-      <c r="C143" s="9"/>
+      <c r="A143" s="16"/>
+      <c r="B143" s="16"/>
+      <c r="C143" s="16"/>
     </row>
     <row r="144" spans="1:4">
-      <c r="A144" s="9" t="s">
+      <c r="A144" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="B144" s="9" t="s">
+      <c r="B144" s="16" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="145" spans="1:4">
-      <c r="A145" s="9"/>
-      <c r="B145" s="9"/>
+      <c r="A145" s="16"/>
+      <c r="B145" s="16"/>
     </row>
     <row r="146" spans="1:4" ht="17">
-      <c r="A146" s="9"/>
-      <c r="B146" s="9"/>
+      <c r="A146" s="16"/>
+      <c r="B146" s="16"/>
       <c r="C146" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:4">
-      <c r="A147" s="9"/>
-      <c r="B147" s="9"/>
+      <c r="A147" s="16"/>
+      <c r="B147" s="16"/>
     </row>
     <row r="148" spans="1:4">
-      <c r="A148" s="9" t="s">
+      <c r="A148" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="B148" s="9" t="s">
+      <c r="B148" s="16" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="149" spans="1:4">
-      <c r="A149" s="9"/>
-      <c r="B149" s="9"/>
+      <c r="A149" s="16"/>
+      <c r="B149" s="16"/>
     </row>
     <row r="150" spans="1:4" ht="17">
-      <c r="A150" s="9"/>
-      <c r="B150" s="9"/>
+      <c r="A150" s="16"/>
+      <c r="B150" s="16"/>
       <c r="C150" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:4">
-      <c r="A151" s="9"/>
-      <c r="B151" s="9"/>
+      <c r="A151" s="16"/>
+      <c r="B151" s="16"/>
     </row>
     <row r="152" spans="1:4">
-      <c r="A152" s="9" t="s">
+      <c r="A152" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B152" s="9" t="s">
+      <c r="B152" s="16" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="153" spans="1:4">
-      <c r="A153" s="9"/>
-      <c r="B153" s="9"/>
+      <c r="A153" s="16"/>
+      <c r="B153" s="16"/>
     </row>
     <row r="154" spans="1:4" ht="17">
-      <c r="A154" s="9"/>
-      <c r="B154" s="9"/>
+      <c r="A154" s="16"/>
+      <c r="B154" s="16"/>
       <c r="C154" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:4">
-      <c r="A155" s="9"/>
-      <c r="B155" s="9"/>
+      <c r="A155" s="16"/>
+      <c r="B155" s="16"/>
     </row>
     <row r="156" spans="1:4">
-      <c r="A156" s="9"/>
-      <c r="B156" s="9"/>
+      <c r="A156" s="16"/>
+      <c r="B156" s="16"/>
     </row>
     <row r="157" spans="1:4">
-      <c r="A157" s="9" t="s">
+      <c r="A157" s="16" t="s">
         <v>111</v>
       </c>
-      <c r="B157" s="9" t="s">
+      <c r="B157" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="C157" s="9" t="s">
+      <c r="C157" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="D157" s="10"/>
+      <c r="D157" s="17"/>
     </row>
     <row r="158" spans="1:4">
-      <c r="A158" s="9"/>
-      <c r="B158" s="9"/>
-      <c r="C158" s="9"/>
-      <c r="D158" s="10"/>
+      <c r="A158" s="16"/>
+      <c r="B158" s="16"/>
+      <c r="C158" s="16"/>
+      <c r="D158" s="17"/>
     </row>
     <row r="160" spans="1:4" ht="18">
       <c r="A160" s="3" t="s">
@@ -5688,110 +5733,110 @@
       </c>
     </row>
     <row r="162" spans="1:4">
-      <c r="A162" s="11" t="s">
+      <c r="A162" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B162" s="11" t="s">
+      <c r="B162" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="D162" s="11" t="s">
+      <c r="D162" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:4">
-      <c r="A163" s="11"/>
-      <c r="B163" s="11"/>
-      <c r="D163" s="11"/>
+      <c r="A163" s="15"/>
+      <c r="B163" s="15"/>
+      <c r="D163" s="15"/>
     </row>
     <row r="164" spans="1:4" ht="17">
-      <c r="A164" s="11"/>
-      <c r="B164" s="11"/>
+      <c r="A164" s="15"/>
+      <c r="B164" s="15"/>
       <c r="C164" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D164" s="11"/>
+      <c r="D164" s="15"/>
     </row>
     <row r="165" spans="1:4">
-      <c r="A165" s="11"/>
-      <c r="B165" s="11"/>
-      <c r="D165" s="11"/>
+      <c r="A165" s="15"/>
+      <c r="B165" s="15"/>
+      <c r="D165" s="15"/>
     </row>
     <row r="166" spans="1:4">
-      <c r="A166" s="11"/>
-      <c r="B166" s="11"/>
-      <c r="D166" s="11"/>
+      <c r="A166" s="15"/>
+      <c r="B166" s="15"/>
+      <c r="D166" s="15"/>
     </row>
     <row r="167" spans="1:4">
-      <c r="A167" s="9" t="s">
+      <c r="A167" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B167" s="9" t="s">
+      <c r="B167" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C167" s="9" t="s">
+      <c r="C167" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D167" s="10"/>
+      <c r="D167" s="17"/>
     </row>
     <row r="168" spans="1:4">
-      <c r="A168" s="9"/>
-      <c r="B168" s="9"/>
-      <c r="C168" s="9"/>
-      <c r="D168" s="10"/>
+      <c r="A168" s="16"/>
+      <c r="B168" s="16"/>
+      <c r="C168" s="16"/>
+      <c r="D168" s="17"/>
     </row>
     <row r="169" spans="1:4">
-      <c r="A169" s="9" t="s">
+      <c r="A169" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="B169" s="9" t="s">
+      <c r="B169" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="C169" s="9" t="s">
+      <c r="C169" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D169" s="10"/>
+      <c r="D169" s="17"/>
     </row>
     <row r="170" spans="1:4">
-      <c r="A170" s="9"/>
-      <c r="B170" s="9"/>
-      <c r="C170" s="9"/>
-      <c r="D170" s="10"/>
+      <c r="A170" s="16"/>
+      <c r="B170" s="16"/>
+      <c r="C170" s="16"/>
+      <c r="D170" s="17"/>
     </row>
     <row r="171" spans="1:4">
-      <c r="A171" s="9" t="s">
+      <c r="A171" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="B171" s="9" t="s">
+      <c r="B171" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="C171" s="9" t="s">
+      <c r="C171" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="D171" s="10"/>
+      <c r="D171" s="17"/>
     </row>
     <row r="172" spans="1:4">
-      <c r="A172" s="9"/>
-      <c r="B172" s="9"/>
-      <c r="C172" s="9"/>
-      <c r="D172" s="10"/>
+      <c r="A172" s="16"/>
+      <c r="B172" s="16"/>
+      <c r="C172" s="16"/>
+      <c r="D172" s="17"/>
     </row>
     <row r="173" spans="1:4">
-      <c r="A173" s="9" t="s">
+      <c r="A173" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B173" s="9" t="s">
+      <c r="B173" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="C173" s="9" t="s">
+      <c r="C173" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D173" s="10"/>
+      <c r="D173" s="17"/>
     </row>
     <row r="174" spans="1:4">
-      <c r="A174" s="9"/>
-      <c r="B174" s="9"/>
-      <c r="C174" s="9"/>
-      <c r="D174" s="10"/>
+      <c r="A174" s="16"/>
+      <c r="B174" s="16"/>
+      <c r="C174" s="16"/>
+      <c r="D174" s="17"/>
     </row>
     <row r="176" spans="1:4" ht="52">
       <c r="A176" s="5" t="s">
@@ -5829,12 +5874,12 @@
       </c>
     </row>
     <row r="199" spans="1:4" ht="18">
-      <c r="A199" s="13" t="s">
+      <c r="A199" s="10" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="200" spans="1:4">
-      <c r="A200" s="14" t="s">
+      <c r="A200" s="11" t="s">
         <v>129</v>
       </c>
     </row>
@@ -5891,45 +5936,113 @@
     </row>
   </sheetData>
   <mergeCells count="170">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="D10:D13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="B27:B31"/>
-    <mergeCell ref="D27:D31"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="C22:C24"/>
-    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="A173:A174"/>
+    <mergeCell ref="B173:B174"/>
+    <mergeCell ref="C173:C174"/>
+    <mergeCell ref="D173:D174"/>
+    <mergeCell ref="A169:A170"/>
+    <mergeCell ref="B169:B170"/>
+    <mergeCell ref="C169:C170"/>
+    <mergeCell ref="D169:D170"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="B171:B172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="D171:D172"/>
+    <mergeCell ref="A162:A166"/>
+    <mergeCell ref="B162:B166"/>
+    <mergeCell ref="D162:D166"/>
+    <mergeCell ref="A167:A168"/>
+    <mergeCell ref="B167:B168"/>
+    <mergeCell ref="C167:C168"/>
+    <mergeCell ref="D167:D168"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="B152:B156"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="B157:B158"/>
+    <mergeCell ref="C157:C158"/>
+    <mergeCell ref="D157:D158"/>
+    <mergeCell ref="A142:A143"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="A144:A147"/>
+    <mergeCell ref="B144:B147"/>
+    <mergeCell ref="A148:A151"/>
+    <mergeCell ref="B148:B151"/>
+    <mergeCell ref="A136:A138"/>
+    <mergeCell ref="B136:B138"/>
+    <mergeCell ref="C136:C138"/>
+    <mergeCell ref="A139:A141"/>
+    <mergeCell ref="B139:B141"/>
+    <mergeCell ref="C139:C141"/>
+    <mergeCell ref="D123:D126"/>
+    <mergeCell ref="A127:A130"/>
+    <mergeCell ref="B127:B130"/>
+    <mergeCell ref="D127:D130"/>
+    <mergeCell ref="A131:A135"/>
+    <mergeCell ref="B131:B135"/>
+    <mergeCell ref="A116:A117"/>
+    <mergeCell ref="B116:B117"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="B118:B119"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="B123:B126"/>
+    <mergeCell ref="A106:A111"/>
+    <mergeCell ref="B106:B111"/>
+    <mergeCell ref="C106:C111"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B112:B113"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="D99:D100"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="B104:B105"/>
+    <mergeCell ref="C104:C105"/>
+    <mergeCell ref="D104:D105"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="A92:A96"/>
+    <mergeCell ref="B92:B96"/>
+    <mergeCell ref="D92:D96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="D97:D98"/>
+    <mergeCell ref="A81:A83"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="C81:C83"/>
+    <mergeCell ref="A84:A87"/>
+    <mergeCell ref="B84:B87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A76:A80"/>
+    <mergeCell ref="B76:B80"/>
+    <mergeCell ref="D76:D80"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="D67:D68"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="D69:D73"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="A64:A66"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="C64:C66"/>
+    <mergeCell ref="D64:D66"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:C50"/>
+    <mergeCell ref="A51:A55"/>
+    <mergeCell ref="B51:B55"/>
+    <mergeCell ref="D51:D55"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B44:B45"/>
     <mergeCell ref="C44:C45"/>
@@ -5954,113 +6067,45 @@
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="B34:B35"/>
     <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="A64:A66"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="C64:C66"/>
-    <mergeCell ref="D64:D66"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:C50"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="B51:B55"/>
-    <mergeCell ref="D51:D55"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="A76:A80"/>
-    <mergeCell ref="B76:B80"/>
-    <mergeCell ref="D76:D80"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="D69:D73"/>
-    <mergeCell ref="A81:A83"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="C81:C83"/>
-    <mergeCell ref="A84:A87"/>
-    <mergeCell ref="B84:B87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D99:D100"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="B104:B105"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="D104:D105"/>
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="A92:A96"/>
-    <mergeCell ref="B92:B96"/>
-    <mergeCell ref="D92:D96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="D97:D98"/>
-    <mergeCell ref="A106:A111"/>
-    <mergeCell ref="B106:B111"/>
-    <mergeCell ref="C106:C111"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B112:B113"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="D123:D126"/>
-    <mergeCell ref="A127:A130"/>
-    <mergeCell ref="B127:B130"/>
-    <mergeCell ref="D127:D130"/>
-    <mergeCell ref="A131:A135"/>
-    <mergeCell ref="B131:B135"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="B116:B117"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="B118:B119"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="B123:B126"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="B142:B143"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="A144:A147"/>
-    <mergeCell ref="B144:B147"/>
-    <mergeCell ref="A148:A151"/>
-    <mergeCell ref="B148:B151"/>
-    <mergeCell ref="A136:A138"/>
-    <mergeCell ref="B136:B138"/>
-    <mergeCell ref="C136:C138"/>
-    <mergeCell ref="A139:A141"/>
-    <mergeCell ref="B139:B141"/>
-    <mergeCell ref="C139:C141"/>
-    <mergeCell ref="A162:A166"/>
-    <mergeCell ref="B162:B166"/>
-    <mergeCell ref="D162:D166"/>
-    <mergeCell ref="A167:A168"/>
-    <mergeCell ref="B167:B168"/>
-    <mergeCell ref="C167:C168"/>
-    <mergeCell ref="D167:D168"/>
-    <mergeCell ref="A152:A156"/>
-    <mergeCell ref="B152:B156"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="B157:B158"/>
-    <mergeCell ref="C157:C158"/>
-    <mergeCell ref="D157:D158"/>
-    <mergeCell ref="A173:A174"/>
-    <mergeCell ref="B173:B174"/>
-    <mergeCell ref="C173:C174"/>
-    <mergeCell ref="D173:D174"/>
-    <mergeCell ref="A169:A170"/>
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="C169:C170"/>
-    <mergeCell ref="D169:D170"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="B171:B172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="D171:D172"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B31"/>
+    <mergeCell ref="D27:D31"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="D10:D13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6069,61 +6114,74 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8216F98-DF56-724A-A913-28E53FD6273C}">
-  <dimension ref="A2:L15"/>
+  <dimension ref="A2:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="32.1640625" style="1" customWidth="1"/>
     <col min="2" max="3" width="13.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="1" customWidth="1"/>
-    <col min="6" max="12" width="10.83203125" style="1"/>
+    <col min="4" max="5" width="13.1640625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="26.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" style="1" customWidth="1"/>
+    <col min="8" max="14" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" s="15" customFormat="1" ht="17">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:14" s="12" customFormat="1" ht="34">
+      <c r="A2" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="G2" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-    </row>
-    <row r="3" spans="1:12" ht="51">
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+    <row r="3" spans="1:14" ht="51">
       <c r="A3" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="68">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:14" ht="68">
+      <c r="A4" s="14" t="s">
         <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -6132,11 +6190,17 @@
       <c r="C4" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="34">
+    <row r="5" spans="1:14" ht="34">
       <c r="A5" s="1" t="s">
         <v>152</v>
       </c>
@@ -6146,47 +6210,85 @@
       <c r="C5" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="17">
+    <row r="6" spans="1:14" ht="17">
       <c r="A6" s="1" t="s">
         <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="34">
+    <row r="7" spans="1:14" ht="34">
       <c r="A7" s="1" t="s">
         <v>159</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="34">
+    <row r="8" spans="1:14" ht="17">
+      <c r="A8" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="34">
       <c r="A12" s="1" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="34">
+    <row r="15" spans="1:14" ht="34">
       <c r="A15" s="1" t="s">
         <v>168</v>
       </c>

</xml_diff>